<commit_message>
percentage:: by sergio giraldo @ 20230305T2145CET, gpg signed
</commit_message>
<xml_diff>
--- a/excel/Basic_Functions.xlsx
+++ b/excel/Basic_Functions.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/GK47LX/source/office/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95941E81-2948-C447-8FC2-29E8347F5988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE460B2B-A86C-7A43-AA94-F65A388FCA90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" xr2:uid="{0ACB132C-7219-4B66-ACBB-64BA10C47BDC}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" activeTab="1" xr2:uid="{0ACB132C-7219-4B66-ACBB-64BA10C47BDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Functions" sheetId="3" r:id="rId1"/>
+    <sheet name="DOING PERCENTAGE CORRECTLY" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="108">
   <si>
     <t>Name</t>
   </si>
@@ -278,22 +279,121 @@
     <t>Column reference is locked but row changes</t>
   </si>
   <si>
-    <t>WHAT HAPPENS WHEN YOU DRAG A FORMULA WITH $ (DOLLAR SIGN)</t>
+    <t>Percentage Change</t>
+  </si>
+  <si>
+    <t>Sales Values</t>
+  </si>
+  <si>
+    <t>App</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Budget</t>
+  </si>
+  <si>
+    <t>% Change</t>
+  </si>
+  <si>
+    <t>WenCaL</t>
+  </si>
+  <si>
+    <t>Blend</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>Inkly</t>
+  </si>
+  <si>
+    <t>Sleops</t>
+  </si>
+  <si>
+    <t>Kind Ape</t>
+  </si>
+  <si>
+    <t>Pet Feed</t>
+  </si>
+  <si>
+    <t>Right App</t>
+  </si>
+  <si>
+    <t>Mirrrr</t>
+  </si>
+  <si>
+    <t>Halotot</t>
+  </si>
+  <si>
+    <t>Flowrrr</t>
+  </si>
+  <si>
+    <t>Silvrr</t>
+  </si>
+  <si>
+    <t>Starting Price</t>
+  </si>
+  <si>
+    <t>End Price</t>
+  </si>
+  <si>
+    <t>2. INTERNALLY, A PERCENTAGE CELL IS A DECIMAL BETWEEN 0 AND 1</t>
+  </si>
+  <si>
+    <t>ALWAYS REMEMBER TO PLUS-1/MINUS-1 THE PERCENTAGE VALUES</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. FORMAT YOUR CELL AS PERCENTAGE </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BEFORE MAKING THE FORMULA</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Apply Percentage </t>
+  </si>
+  <si>
+    <t>Change Price by</t>
+  </si>
+  <si>
+    <t>WHEN YOU WRITE THE CELL REFERENCE, PRESS F4 TO INSERT THE DOLLAR SIGN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHAT HAPPENS WHEN YOU DRAG A FORMULA WITH $ (DOLLAR SIGN). </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="* #,##0.00;_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="174" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="170" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="15">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -357,16 +457,66 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -496,98 +646,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="174" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="1" fillId="2" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="10">
     <cellStyle name="Comma" xfId="7" builtinId="3"/>
     <cellStyle name="Heading 1 2" xfId="5" xr:uid="{B6C151E3-A0C4-4A2F-BB0C-BAB9428B5FF7}"/>
+    <cellStyle name="Heading 2" xfId="9" builtinId="17"/>
     <cellStyle name="Heading 2 2" xfId="6" xr:uid="{1F4E3DA3-A240-45F6-A5B7-6EE24E59192F}"/>
     <cellStyle name="Heading green" xfId="4" xr:uid="{D92394D5-776D-4DDF-BD60-D8FC3AAF15BD}"/>
     <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{C7222ADA-7BFB-4211-ADD4-320EDB0CA053}"/>
     <cellStyle name="Hyperlink 3" xfId="3" xr:uid="{6B1C1235-260E-4EE2-9B1B-D7D7663FC318}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{B44826F6-5397-47E2-B941-E5B9A5628A85}"/>
+    <cellStyle name="Per cent" xfId="8" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -899,10 +1119,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F5FC3B6-D4BB-4A90-B4D4-E75BB2C1D935}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -1006,7 +1226,6 @@
       <c r="E4" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="16"/>
       <c r="G4" s="1" t="s">
         <v>52</v>
       </c>
@@ -1034,7 +1253,6 @@
       <c r="E5" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="16"/>
       <c r="G5" s="2" t="s">
         <v>16</v>
       </c>
@@ -1063,7 +1281,6 @@
       <c r="E6" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="16"/>
       <c r="G6" s="2" t="s">
         <v>42</v>
       </c>
@@ -1071,10 +1288,10 @@
         <f>COUNT(E3:E11)</f>
         <v>4</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="18"/>
+      <c r="J6" s="17"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="10" t="s">
@@ -1089,7 +1306,7 @@
       <c r="D7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="15" t="s">
         <v>41</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -1102,7 +1319,7 @@
       <c r="I7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="18"/>
+      <c r="J7" s="17"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="10" t="s">
@@ -1117,7 +1334,7 @@
       <c r="D8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="15">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -1127,10 +1344,10 @@
         <f>COUNTA(E3:E11)</f>
         <v>9</v>
       </c>
-      <c r="I8" s="17" t="s">
+      <c r="I8" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="20"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="10" t="s">
@@ -1145,7 +1362,7 @@
       <c r="D9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="19">
+      <c r="E9" s="15">
         <v>2</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -1155,10 +1372,10 @@
         <f>MIN(C3:C11)</f>
         <v>29727</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="J9" s="20"/>
+      <c r="J9" s="18"/>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="10" t="s">
@@ -1173,32 +1390,32 @@
       <c r="D10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="15">
         <v>3</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="19">
         <f>_xlfn.MINIFS(C3:C11,B3:B11,"Sales")</f>
         <v>34808</v>
       </c>
       <c r="I10" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="J10" s="18"/>
+      <c r="J10" s="17"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="11">
         <v>32761</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="10" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="15">
@@ -1211,7 +1428,7 @@
         <f>MAX(C3:C11)</f>
         <v>134468</v>
       </c>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="17" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1223,7 +1440,7 @@
         <f>COUNTIFS(B3:C11,"Sales")</f>
         <v>4</v>
       </c>
-      <c r="I12" s="20" t="s">
+      <c r="I12" s="18" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1235,7 +1452,7 @@
         <f>SUMIFS(C3:C11,D3:D11,"MI")</f>
         <v>206405</v>
       </c>
-      <c r="I13" s="20" t="s">
+      <c r="I13" s="18" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1243,11 +1460,11 @@
       <c r="G14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="24">
+      <c r="H14" s="20">
         <f>AVERAGEIFS(C3:C11,B3:B11,"Sales")</f>
         <v>75642.75</v>
       </c>
-      <c r="I14" s="18" t="s">
+      <c r="I14" s="17" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1259,415 +1476,773 @@
         <f>COUNTA(_xlfn.UNIQUE(B3:B11))</f>
         <v>3</v>
       </c>
-      <c r="I15" s="20" t="s">
+      <c r="I15" s="18" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="19" spans="3:9">
-      <c r="C19" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
+      <c r="C19" s="56" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
     </row>
     <row r="20" spans="3:9">
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+    </row>
+    <row r="21" spans="3:9">
+      <c r="C21" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D21" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E21" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="29"/>
-    </row>
-    <row r="21" spans="3:9">
-      <c r="C21" s="30">
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="24"/>
+    </row>
+    <row r="22" spans="3:9">
+      <c r="C22" s="25">
         <v>100</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D22" s="1">
         <v>3</v>
       </c>
-      <c r="E21" s="31">
-        <f>C21+D21</f>
+      <c r="E22" s="1">
+        <f>C22+D22</f>
         <v>103</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F22" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="31" t="s">
+      <c r="G22" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H21" s="31"/>
-      <c r="I21" s="33"/>
-    </row>
-    <row r="22" spans="3:9">
-      <c r="C22" s="30">
+      <c r="I22" s="26"/>
+    </row>
+    <row r="23" spans="3:9">
+      <c r="C23" s="25">
         <v>1</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D23" s="1">
         <v>4</v>
       </c>
-      <c r="E22" s="31">
-        <f t="shared" ref="E22:E24" si="0">C22+D22</f>
+      <c r="E23" s="1">
+        <f t="shared" ref="E23:E25" si="0">C23+D23</f>
         <v>5</v>
       </c>
-      <c r="F22" s="32" t="s">
+      <c r="F23" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="33"/>
-    </row>
-    <row r="23" spans="3:9">
-      <c r="C23" s="30">
+      <c r="I23" s="26"/>
+    </row>
+    <row r="24" spans="3:9">
+      <c r="C24" s="25">
         <v>2</v>
       </c>
-      <c r="D23" s="31">
+      <c r="D24" s="1">
         <v>5</v>
       </c>
-      <c r="E23" s="31">
+      <c r="E24" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="F23" s="32" t="s">
+      <c r="F24" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="33"/>
-    </row>
-    <row r="24" spans="3:9">
-      <c r="C24" s="30">
+      <c r="I24" s="26"/>
+    </row>
+    <row r="25" spans="3:9">
+      <c r="C25" s="25">
         <v>2</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D25" s="1">
         <v>6</v>
       </c>
-      <c r="E24" s="31">
+      <c r="E25" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F24" s="32" t="s">
+      <c r="F25" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="33"/>
-    </row>
-    <row r="25" spans="3:9">
-      <c r="C25" s="30"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="33"/>
+      <c r="I25" s="26"/>
     </row>
     <row r="26" spans="3:9">
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="25"/>
+      <c r="I26" s="26"/>
+    </row>
+    <row r="27" spans="3:9">
+      <c r="C27" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D27" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="E26" s="35" t="s">
+      <c r="E27" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="F26" s="31"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="33"/>
-    </row>
-    <row r="27" spans="3:9">
-      <c r="C27" s="36">
+      <c r="I27" s="26"/>
+    </row>
+    <row r="28" spans="3:9">
+      <c r="C28" s="29">
         <v>100</v>
       </c>
-      <c r="D27" s="37">
+      <c r="D28" s="30">
         <v>3</v>
       </c>
-      <c r="E27" s="37">
-        <f>$C$27+D27</f>
+      <c r="E28" s="30">
+        <f>$C$28+D28</f>
         <v>103</v>
       </c>
-      <c r="F27" s="38" t="s">
+      <c r="F28" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="G27" s="31" t="s">
+      <c r="G28" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="H27" s="31"/>
-      <c r="I27" s="33"/>
-    </row>
-    <row r="28" spans="3:9">
-      <c r="C28" s="36">
+      <c r="I28" s="26"/>
+    </row>
+    <row r="29" spans="3:9">
+      <c r="C29" s="29">
         <v>1</v>
       </c>
-      <c r="D28" s="37">
+      <c r="D29" s="30">
         <v>4</v>
       </c>
-      <c r="E28" s="37">
-        <f t="shared" ref="E28:E30" si="1">$C$27+D28</f>
+      <c r="E29" s="30">
+        <f t="shared" ref="E29:E31" si="1">$C$28+D29</f>
         <v>104</v>
       </c>
-      <c r="F28" s="38" t="s">
+      <c r="F29" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="31" t="s">
+      <c r="G29" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H28" s="31"/>
-      <c r="I28" s="33"/>
-    </row>
-    <row r="29" spans="3:9">
-      <c r="C29" s="36">
+      <c r="I29" s="26"/>
+    </row>
+    <row r="30" spans="3:9">
+      <c r="C30" s="29">
         <v>2</v>
       </c>
-      <c r="D29" s="37">
+      <c r="D30" s="30">
         <v>5</v>
       </c>
-      <c r="E29" s="37">
+      <c r="E30" s="30">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="F29" s="38" t="s">
+      <c r="F30" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="33"/>
-    </row>
-    <row r="30" spans="3:9">
-      <c r="C30" s="36">
+      <c r="I30" s="26"/>
+    </row>
+    <row r="31" spans="3:9">
+      <c r="C31" s="29">
         <v>2</v>
       </c>
-      <c r="D30" s="37">
+      <c r="D31" s="30">
         <v>6</v>
       </c>
-      <c r="E30" s="37">
+      <c r="E31" s="30">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
-      <c r="F30" s="38" t="s">
+      <c r="F31" s="31" t="s">
         <v>62</v>
       </c>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="33"/>
-    </row>
-    <row r="31" spans="3:9">
-      <c r="C31" s="30"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="33"/>
+      <c r="I31" s="26"/>
     </row>
     <row r="32" spans="3:9">
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="25"/>
+      <c r="I32" s="26"/>
+    </row>
+    <row r="33" spans="3:9">
+      <c r="C33" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="35" t="s">
+      <c r="D33" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="35" t="s">
+      <c r="E33" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="33"/>
-    </row>
-    <row r="33" spans="3:9">
-      <c r="C33" s="36">
+      <c r="I33" s="26"/>
+    </row>
+    <row r="34" spans="3:9">
+      <c r="C34" s="29">
         <v>100</v>
       </c>
-      <c r="D33" s="37">
+      <c r="D34" s="30">
         <v>3</v>
       </c>
-      <c r="E33" s="31">
+      <c r="E34" s="1">
         <v>10</v>
       </c>
-      <c r="F33" s="31">
-        <f>C$33+D33+E33</f>
+      <c r="F34" s="1">
+        <f>C$34+D34+E34</f>
         <v>113</v>
       </c>
-      <c r="G33" s="31">
-        <f>D$33+E33+F33</f>
+      <c r="G34" s="1">
+        <f>D$34+E34+F34</f>
         <v>126</v>
       </c>
-      <c r="H33" s="31">
-        <f>E$33+F33+G33</f>
+      <c r="H34" s="1">
+        <f>E$34+F34+G34</f>
         <v>249</v>
       </c>
-      <c r="I33" s="33" t="s">
+      <c r="I34" s="26" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="3:9">
-      <c r="C34" s="36"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="32" t="s">
+    <row r="35" spans="3:9">
+      <c r="C35" s="29"/>
+      <c r="D35" s="30"/>
+      <c r="F35" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="G34" s="39" t="s">
+      <c r="G35" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="H34" s="32" t="s">
+      <c r="H35" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="I34" s="33" t="s">
+      <c r="I35" s="26" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="3:9">
-      <c r="C35" s="36"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="33"/>
-    </row>
     <row r="36" spans="3:9">
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="29"/>
+      <c r="D36" s="30"/>
+      <c r="I36" s="26"/>
+    </row>
+    <row r="37" spans="3:9">
+      <c r="C37" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D37" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="33"/>
-    </row>
-    <row r="37" spans="3:9">
-      <c r="C37" s="30">
+      <c r="I37" s="26"/>
+    </row>
+    <row r="38" spans="3:9">
+      <c r="C38" s="25">
         <v>1</v>
       </c>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="33"/>
-    </row>
-    <row r="38" spans="3:9">
-      <c r="C38" s="30">
+      <c r="I38" s="26"/>
+    </row>
+    <row r="39" spans="3:9">
+      <c r="C39" s="25">
         <v>2</v>
       </c>
-      <c r="D38" s="31">
-        <f>$C37+$C38</f>
+      <c r="D39" s="1">
+        <f>$C38+$C39</f>
         <v>3</v>
       </c>
-      <c r="E38" s="32" t="s">
+      <c r="E39" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="F38" s="31"/>
-      <c r="G38" s="31" t="s">
+      <c r="G39" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H38" s="31"/>
-      <c r="I38" s="33"/>
-    </row>
-    <row r="39" spans="3:9">
-      <c r="C39" s="30">
+      <c r="I39" s="26"/>
+    </row>
+    <row r="40" spans="3:9">
+      <c r="C40" s="25">
         <v>3</v>
       </c>
-      <c r="D39" s="31">
-        <f t="shared" ref="D39:D42" si="2">$C38+$C39</f>
+      <c r="D40" s="1">
+        <f t="shared" ref="D40:D43" si="2">$C39+$C40</f>
         <v>5</v>
       </c>
-      <c r="E39" s="32" t="s">
+      <c r="E40" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="F39" s="31"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="31"/>
-      <c r="I39" s="33"/>
-    </row>
-    <row r="40" spans="3:9">
-      <c r="C40" s="30">
+      <c r="I40" s="26"/>
+    </row>
+    <row r="41" spans="3:9">
+      <c r="C41" s="25">
         <v>4</v>
       </c>
-      <c r="D40" s="31">
+      <c r="D41" s="1">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="E40" s="32" t="s">
+      <c r="E41" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="33"/>
-    </row>
-    <row r="41" spans="3:9">
-      <c r="C41" s="30">
+      <c r="I41" s="26"/>
+    </row>
+    <row r="42" spans="3:9">
+      <c r="C42" s="25">
         <v>5</v>
       </c>
-      <c r="D41" s="31">
+      <c r="D42" s="1">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="E41" s="32" t="s">
+      <c r="E42" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="33"/>
-    </row>
-    <row r="42" spans="3:9">
-      <c r="C42" s="40">
+      <c r="I42" s="26"/>
+    </row>
+    <row r="43" spans="3:9">
+      <c r="C43" s="33">
         <v>6</v>
       </c>
-      <c r="D42" s="41">
+      <c r="D43" s="34">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="E42" s="42" t="s">
+      <c r="E43" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="F42" s="41"/>
-      <c r="G42" s="41"/>
-      <c r="H42" s="41"/>
-      <c r="I42" s="43"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="34"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="C20:I20"/>
     <mergeCell ref="C19:I19"/>
   </mergeCells>
-  <phoneticPr fontId="7" type="noConversion"/>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC63271-1EF2-244B-AF39-044CFD15E20E}">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="10.1640625" style="40"/>
+    <col min="2" max="2" width="12.33203125" style="40" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="40" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" style="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.1640625" style="40"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="38" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="G2" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+    </row>
+    <row r="3" spans="1:12" ht="17">
+      <c r="B3" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="41"/>
+    </row>
+    <row r="4" spans="1:12" ht="18" thickBot="1">
+      <c r="A4" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="45">
+        <v>14432</v>
+      </c>
+      <c r="C5" s="45">
+        <v>15113</v>
+      </c>
+      <c r="D5" s="51">
+        <f>B5/C5-1</f>
+        <v>-4.5060543902600392E-2</v>
+      </c>
+      <c r="E5" s="50" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(D5)</f>
+        <v>=B5/C5-1</v>
+      </c>
+      <c r="G5" s="50" t="s">
+        <v>102</v>
+      </c>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="50"/>
+      <c r="K5" s="50"/>
+      <c r="L5" s="50"/>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="45">
+        <v>17990</v>
+      </c>
+      <c r="C6" s="45">
+        <v>18181</v>
+      </c>
+      <c r="D6" s="51">
+        <f t="shared" ref="D6:D16" si="0">B6/C6-1</f>
+        <v>-1.0505472746273559E-2</v>
+      </c>
+      <c r="E6" s="50" t="str">
+        <f t="shared" ref="E6:E16" ca="1" si="1">_xlfn.FORMULATEXT(D6)</f>
+        <v>=B6/C6-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="40" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="45">
+        <v>15117</v>
+      </c>
+      <c r="C7" s="45">
+        <v>13455</v>
+      </c>
+      <c r="D7" s="51">
+        <f t="shared" si="0"/>
+        <v>0.12352285395763651</v>
+      </c>
+      <c r="E7" s="50" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=B7/C7-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="45">
+        <v>11154</v>
+      </c>
+      <c r="C8" s="45">
+        <v>12031</v>
+      </c>
+      <c r="D8" s="51">
+        <f t="shared" si="0"/>
+        <v>-7.2895021195245602E-2</v>
+      </c>
+      <c r="E8" s="50" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=B8/C8-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" s="45">
+        <v>11022</v>
+      </c>
+      <c r="C9" s="45">
+        <v>14600</v>
+      </c>
+      <c r="D9" s="51">
+        <f t="shared" si="0"/>
+        <v>-0.24506849315068491</v>
+      </c>
+      <c r="E9" s="50" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=B9/C9-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="45">
+        <v>8905</v>
+      </c>
+      <c r="C10" s="45">
+        <v>9096</v>
+      </c>
+      <c r="D10" s="51">
+        <f t="shared" si="0"/>
+        <v>-2.0998240985048322E-2</v>
+      </c>
+      <c r="E10" s="50" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=B10/C10-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="45">
+        <v>16735</v>
+      </c>
+      <c r="C11" s="45">
+        <v>18207</v>
+      </c>
+      <c r="D11" s="51">
+        <f t="shared" si="0"/>
+        <v>-8.0848025484703712E-2</v>
+      </c>
+      <c r="E11" s="50" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=B11/C11-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="45">
+        <v>3635</v>
+      </c>
+      <c r="C12" s="45">
+        <v>3579</v>
+      </c>
+      <c r="D12" s="51">
+        <f t="shared" si="0"/>
+        <v>1.5646828723107076E-2</v>
+      </c>
+      <c r="E12" s="50" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=B12/C12-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="40" t="s">
+        <v>95</v>
+      </c>
+      <c r="B13" s="45">
+        <v>15627</v>
+      </c>
+      <c r="C13" s="45">
+        <v>14634</v>
+      </c>
+      <c r="D13" s="51">
+        <f t="shared" si="0"/>
+        <v>6.7855678556785648E-2</v>
+      </c>
+      <c r="E13" s="50" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=B13/C13-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="45">
+        <v>7270</v>
+      </c>
+      <c r="C14" s="45">
+        <v>7158</v>
+      </c>
+      <c r="D14" s="51">
+        <f t="shared" si="0"/>
+        <v>1.5646828723107076E-2</v>
+      </c>
+      <c r="E14" s="50" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=B14/C14-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" s="45">
+        <v>5955</v>
+      </c>
+      <c r="C15" s="45">
+        <v>5977</v>
+      </c>
+      <c r="D15" s="51">
+        <f t="shared" si="0"/>
+        <v>-3.6807763091851742E-3</v>
+      </c>
+      <c r="E15" s="50" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=B15/C15-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="45">
+        <v>7666</v>
+      </c>
+      <c r="C16" s="45">
+        <v>7099</v>
+      </c>
+      <c r="D16" s="51">
+        <f t="shared" si="0"/>
+        <v>7.9870404282293306E-2</v>
+      </c>
+      <c r="E16" s="50" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>=B16/C16-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="E17" s="54"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+    </row>
+    <row r="19" spans="1:5" ht="35" thickBot="1">
+      <c r="A19" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="40">
+        <v>100</v>
+      </c>
+      <c r="B20" s="52">
+        <v>0.1</v>
+      </c>
+      <c r="C20" s="46">
+        <f>A20*(1+B20)</f>
+        <v>110.00000000000001</v>
+      </c>
+      <c r="D20" s="50" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(C20)</f>
+        <v>=A20*(1+B20)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="40">
+        <v>50</v>
+      </c>
+      <c r="B21" s="52">
+        <v>-0.2</v>
+      </c>
+      <c r="C21" s="46">
+        <f t="shared" ref="C21:C23" si="2">A21*(1+B21)</f>
+        <v>40</v>
+      </c>
+      <c r="D21" s="50" t="str">
+        <f t="shared" ref="D21:D23" ca="1" si="3">_xlfn.FORMULATEXT(C21)</f>
+        <v>=A21*(1+B21)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="40">
+        <v>80</v>
+      </c>
+      <c r="B22" s="52">
+        <v>0.05</v>
+      </c>
+      <c r="C22" s="46">
+        <f t="shared" si="2"/>
+        <v>84</v>
+      </c>
+      <c r="D22" s="50" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=A22*(1+B22)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="40">
+        <v>20</v>
+      </c>
+      <c r="B23" s="52">
+        <v>0.3</v>
+      </c>
+      <c r="C23" s="46">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="D23" s="50" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>=A23*(1+B23)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" s="53"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="C25" s="55"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1855,18 +2430,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41835CC1-5B38-4C58-812E-EE1DC552CFC3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AF0F56E-77F7-47C1-93E6-4E9B1B632CC3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1AF0F56E-77F7-47C1-93E6-4E9B1B632CC3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41835CC1-5B38-4C58-812E-EE1DC552CFC3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>